<commit_message>
creacion de varias funciones
</commit_message>
<xml_diff>
--- a/Hojas de calculo/Valor k.xlsx
+++ b/Hojas de calculo/Valor k.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/germanlopezpineda/Documents/Python/CargaAdmisible/Hojas de calculo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0AFE331-08DB-9C46-8DB1-1949726998EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA9073C-91E3-CA45-9E24-852C07E0A180}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22420" yWindow="2240" windowWidth="28040" windowHeight="17440" xr2:uid="{FAAB56AC-25BB-B041-8ED8-9B86F85F2AE9}"/>
+    <workbookView xWindow="6520" yWindow="2520" windowWidth="28040" windowHeight="17440" xr2:uid="{FAAB56AC-25BB-B041-8ED8-9B86F85F2AE9}"/>
   </bookViews>
   <sheets>
     <sheet name="K" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>n</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>mm</t>
+  </si>
+  <si>
+    <t>CÁLCULO DE ASIENTOS PARA ESPACIO ELÁSTICO INDEFINIDO</t>
   </si>
 </sst>
 </file>
@@ -224,7 +227,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>K!$B$3</c:f>
+              <c:f>K!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -257,7 +260,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>K!$A$4:$A$25</c:f>
+              <c:f>K!$A$5:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
@@ -332,7 +335,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>K!$B$4:$B$25</c:f>
+              <c:f>K!$B$5:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="22"/>
@@ -764,7 +767,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>K!$B$3</c:f>
+              <c:f>K!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -847,7 +850,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>K!$A$4:$A$25</c:f>
+              <c:f>K!$A$5:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
@@ -922,7 +925,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>K!$B$4:$B$25</c:f>
+              <c:f>K!$B$5:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="22"/>
@@ -1324,7 +1327,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>K!$B$3</c:f>
+              <c:f>K!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1357,7 +1360,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>K!$A$4:$A$25</c:f>
+              <c:f>K!$A$5:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
@@ -1432,7 +1435,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>K!$B$4:$B$25</c:f>
+              <c:f>K!$B$5:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="22"/>
@@ -1517,7 +1520,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>K!$C$3</c:f>
+              <c:f>K!$C$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1550,7 +1553,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>K!$A$4:$A$25</c:f>
+              <c:f>K!$A$5:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
@@ -1625,7 +1628,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>K!$C$4:$C$25</c:f>
+              <c:f>K!$C$5:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="22"/>
@@ -2065,7 +2068,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>K!$B$3</c:f>
+              <c:f>K!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2098,7 +2101,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>K!$A$4:$A$25</c:f>
+              <c:f>K!$A$5:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
@@ -2173,7 +2176,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>K!$C$4:$C$25</c:f>
+              <c:f>K!$C$5:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="22"/>
@@ -4780,13 +4783,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>450850</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>660400</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4816,13 +4819,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>577850</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4854,13 +4857,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4892,13 +4895,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5226,10 +5229,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E1981A-7AC9-1440-8FC8-03D19013AAD0}">
-  <dimension ref="A3:E48"/>
+  <dimension ref="A2:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5239,465 +5242,467 @@
     <col min="3" max="3" width="12.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2">
-        <v>0.56100000000000005</v>
-      </c>
-      <c r="C4" s="2">
-        <f>0.3069*LN(A4)+0.548</f>
-        <v>0.54800000000000004</v>
-      </c>
-      <c r="D4" s="2">
-        <f>B4-C4</f>
-        <v>1.3000000000000012E-2</v>
-      </c>
-      <c r="E4" s="2">
-        <f>D4*100/B4</f>
-        <v>2.3172905525846721</v>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="B5" s="2">
-        <v>0.58799999999999997</v>
+        <v>0.56100000000000005</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" ref="C5:C48" si="0">0.3069*LN(A5)+0.548</f>
-        <v>0.57725069418194741</v>
+        <f>0.3069*LN(A5)+0.548</f>
+        <v>0.54800000000000004</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" ref="D5:D25" si="1">B5-C5</f>
-        <v>1.0749305818052557E-2</v>
+        <f>B5-C5</f>
+        <v>1.3000000000000012E-2</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" ref="E5:E25" si="2">D5*100/B5</f>
-        <v>1.8281132343626798</v>
+        <f>D5*100/B5</f>
+        <v>2.3172905525846721</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>1.2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="B6" s="2">
-        <v>0.61299999999999999</v>
+        <v>0.58799999999999997</v>
       </c>
       <c r="C6" s="2">
-        <f t="shared" si="0"/>
-        <v>0.60395448578006472</v>
+        <f t="shared" ref="C6:C49" si="0">0.3069*LN(A6)+0.548</f>
+        <v>0.57725069418194741</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" si="1"/>
-        <v>9.0455142199352689E-3</v>
+        <f t="shared" ref="D6:D26" si="1">B6-C6</f>
+        <v>1.0749305818052557E-2</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="2"/>
-        <v>1.4756140652422951</v>
+        <f t="shared" ref="E6:E26" si="2">D6*100/B6</f>
+        <v>1.8281132343626798</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="B7" s="2">
-        <v>0.63600000000000001</v>
+        <v>0.61299999999999999</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" si="0"/>
-        <v>0.62851959276507308</v>
+        <v>0.60395448578006472</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="1"/>
-        <v>7.4804072349269335E-3</v>
+        <v>9.0455142199352689E-3</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="2"/>
-        <v>1.1761646595797064</v>
+        <v>1.4756140652422951</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="B8" s="2">
-        <v>0.65800000000000003</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" si="0"/>
-        <v>0.6512633294190503</v>
+        <v>0.62851959276507308</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="1"/>
-        <v>6.7366705809497329E-3</v>
+        <v>7.4804072349269335E-3</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="2"/>
-        <v>1.0238101186853696</v>
+        <v>1.1761646595797064</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="B9" s="2">
-        <v>0.67900000000000005</v>
+        <v>0.65800000000000003</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" si="0"/>
-        <v>0.67243724167839569</v>
+        <v>0.6512633294190503</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="1"/>
-        <v>6.5627583216043561E-3</v>
+        <v>6.7366705809497329E-3</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="2"/>
-        <v>0.9665328897797284</v>
+        <v>1.0238101186853696</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="B10" s="2">
-        <v>0.68899999999999995</v>
+        <v>0.67900000000000005</v>
       </c>
       <c r="C10" s="2">
         <f t="shared" si="0"/>
-        <v>0.69224411381551632</v>
+        <v>0.67243724167839569</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="1"/>
-        <v>-3.2441138155163696E-3</v>
+        <v>6.5627583216043561E-3</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="2"/>
-        <v>-0.4708438048644949</v>
+        <v>0.9665328897797284</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>1.7</v>
+        <v>1.6</v>
       </c>
       <c r="B11" s="2">
-        <v>0.71599999999999997</v>
+        <v>0.68899999999999995</v>
       </c>
       <c r="C11" s="2">
         <f t="shared" si="0"/>
-        <v>0.71084981025098015</v>
+        <v>0.69224411381551632</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="1"/>
-        <v>5.1501897490198179E-3</v>
+        <v>-3.2441138155163696E-3</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" si="2"/>
-        <v>0.71930024427651096</v>
+        <v>-0.4708438048644949</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>1.8</v>
+        <v>1.7</v>
       </c>
       <c r="B12" s="2">
-        <v>0.73399999999999999</v>
+        <v>0.71599999999999997</v>
       </c>
       <c r="C12" s="2">
         <f t="shared" si="0"/>
-        <v>0.72839172745846037</v>
+        <v>0.71084981025098015</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="1"/>
-        <v>5.6082725415396162E-3</v>
+        <v>5.1501897490198179E-3</v>
       </c>
       <c r="E12" s="2">
         <f t="shared" si="2"/>
-        <v>0.76406982854763161</v>
+        <v>0.71930024427651096</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="B13" s="2">
-        <v>0.75</v>
+        <v>0.73399999999999999</v>
       </c>
       <c r="C13" s="2">
         <f t="shared" si="0"/>
-        <v>0.74498495766630801</v>
+        <v>0.72839172745846037</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="1"/>
-        <v>5.015042333691988E-3</v>
+        <v>5.6082725415396162E-3</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="2"/>
-        <v>0.66867231115893178</v>
+        <v>0.76406982854763161</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="B14" s="2">
-        <v>0.76600000000000001</v>
+        <v>0.75</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" si="0"/>
-        <v>0.76072686971384729</v>
+        <v>0.74498495766630801</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="1"/>
-        <v>5.2731302861527274E-3</v>
+        <v>5.015042333691988E-3</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="2"/>
-        <v>0.68839820968051268</v>
+        <v>0.66867231115893178</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="B15" s="2">
-        <v>0.79500000000000004</v>
+        <v>0.76600000000000001</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="0"/>
-        <v>0.78997756389579465</v>
+        <v>0.76072686971384729</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="1"/>
-        <v>5.0224361042053856E-3</v>
+        <v>5.2731302861527274E-3</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="2"/>
-        <v>0.63175296908243839</v>
+        <v>0.68839820968051268</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>2.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B16" s="2">
-        <v>0.82199999999999995</v>
+        <v>0.79500000000000004</v>
       </c>
       <c r="C16" s="2">
         <f t="shared" si="0"/>
-        <v>0.81668135549391185</v>
+        <v>0.78997756389579465</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="1"/>
-        <v>5.3186445060880994E-3</v>
+        <v>5.0224361042053856E-3</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="2"/>
-        <v>0.6470370445362652</v>
+        <v>0.63175296908243839</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>2.6</v>
+        <v>2.4</v>
       </c>
       <c r="B17" s="2">
-        <v>0.84699999999999998</v>
+        <v>0.82199999999999995</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" si="0"/>
-        <v>0.84124646247892021</v>
+        <v>0.81668135549391185</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="1"/>
-        <v>5.7535375210797657E-3</v>
+        <v>5.3186445060880994E-3</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" si="2"/>
-        <v>0.67928424097754025</v>
+        <v>0.6470370445362652</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>2.8</v>
+        <v>2.6</v>
       </c>
       <c r="B18" s="2">
-        <v>0.87</v>
+        <v>0.84699999999999998</v>
       </c>
       <c r="C18" s="2">
         <f t="shared" si="0"/>
-        <v>0.86399019913289754</v>
+        <v>0.84124646247892021</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="1"/>
-        <v>6.009800867102455E-3</v>
+        <v>5.7535375210797657E-3</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" si="2"/>
-        <v>0.69078170886235113</v>
+        <v>0.67928424097754025</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="B19" s="2">
-        <v>0.89200000000000002</v>
+        <v>0.87</v>
       </c>
       <c r="C19" s="2">
         <f t="shared" si="0"/>
-        <v>0.88516411139224294</v>
+        <v>0.86399019913289754</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="1"/>
-        <v>6.8358886077570791E-3</v>
+        <v>6.009800867102455E-3</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" si="2"/>
-        <v>0.7663552250848743</v>
+        <v>0.69078170886235113</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="B20" s="2">
-        <v>0.91200000000000003</v>
+        <v>0.89200000000000002</v>
       </c>
       <c r="C20" s="2">
         <f t="shared" si="0"/>
-        <v>0.90497098352936356</v>
+        <v>0.88516411139224294</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="1"/>
-        <v>7.0290164706364733E-3</v>
+        <v>6.8358886077570791E-3</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" si="2"/>
-        <v>0.7707254902013676</v>
+        <v>0.7663552250848743</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="B21" s="2">
-        <v>0.93100000000000005</v>
+        <v>0.91200000000000003</v>
       </c>
       <c r="C21" s="2">
         <f t="shared" si="0"/>
-        <v>0.92357667996482729</v>
+        <v>0.90497098352936356</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="1"/>
-        <v>7.4233200351727646E-3</v>
+        <v>7.0290164706364733E-3</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" si="2"/>
-        <v>0.79734909078117766</v>
+        <v>0.7707254902013676</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="B22" s="2">
-        <v>0.94899999999999995</v>
+        <v>0.93100000000000005</v>
       </c>
       <c r="C22" s="2">
         <f t="shared" si="0"/>
-        <v>0.9411185971723075</v>
+        <v>0.92357667996482729</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" si="1"/>
-        <v>7.8814028276924519E-3</v>
+        <v>7.4233200351727646E-3</v>
       </c>
       <c r="E22" s="2">
         <f t="shared" si="2"/>
-        <v>0.83049555613197601</v>
+        <v>0.79734909078117766</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="B23" s="2">
-        <v>0.96599999999999997</v>
+        <v>0.94899999999999995</v>
       </c>
       <c r="C23" s="2">
         <f t="shared" si="0"/>
-        <v>0.95771182738015526</v>
+        <v>0.9411185971723075</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" si="1"/>
-        <v>8.2881726198447137E-3</v>
+        <v>7.8814028276924519E-3</v>
       </c>
       <c r="E23" s="2">
         <f t="shared" si="2"/>
-        <v>0.85798888404189588</v>
+        <v>0.83049555613197601</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="B24" s="2">
-        <v>0.98199999999999998</v>
+        <v>0.96599999999999997</v>
       </c>
       <c r="C24" s="2">
         <f t="shared" si="0"/>
-        <v>0.97345373942769453</v>
+        <v>0.95771182738015526</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" si="1"/>
-        <v>8.546260572305453E-3</v>
+        <v>8.2881726198447137E-3</v>
       </c>
       <c r="E24" s="2">
         <f t="shared" si="2"/>
-        <v>0.87029130064210314</v>
+        <v>0.85798888404189588</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25" s="2">
-        <v>1.052</v>
+        <v>0.98199999999999998</v>
       </c>
       <c r="C25" s="2">
         <f t="shared" si="0"/>
-        <v>1.0419364953260255</v>
+        <v>0.97345373942769453</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" si="1"/>
-        <v>1.0063504673974544E-2</v>
+        <v>8.546260572305453E-3</v>
       </c>
       <c r="E25" s="2">
         <f t="shared" si="2"/>
-        <v>0.95660690817248506</v>
+        <v>0.87029130064210314</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C26" s="2"/>
+      <c r="A26" s="1">
+        <v>5</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1.052</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0419364953260255</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0063504673974544E-2</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" si="2"/>
+        <v>0.95660690817248506</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C27" s="2"/>
@@ -5712,41 +5717,30 @@
       <c r="C30" s="2"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31"/>
-      <c r="B31"/>
-      <c r="C31"/>
+      <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32">
-        <v>300</v>
-      </c>
-      <c r="C32" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" t="s">
-        <v>8</v>
-      </c>
+      <c r="A32"/>
+      <c r="B32"/>
+      <c r="C32"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>9</v>
-      </c>
-      <c r="B33" s="3">
-        <v>1.5</v>
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <v>300</v>
       </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B34" s="3">
         <v>1.5</v>
@@ -5755,101 +5749,112 @@
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35"/>
-      <c r="B35"/>
-      <c r="C35"/>
+      <c r="A35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>14</v>
-      </c>
-      <c r="B36">
-        <v>15000</v>
-      </c>
-      <c r="C36" t="s">
-        <v>15</v>
-      </c>
-      <c r="D36" t="s">
-        <v>16</v>
-      </c>
+      <c r="A36"/>
+      <c r="B36"/>
+      <c r="C36"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>17</v>
-      </c>
-      <c r="B37" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="C37"/>
+        <v>14</v>
+      </c>
+      <c r="B37">
+        <v>15000</v>
+      </c>
+      <c r="C37" t="s">
+        <v>15</v>
+      </c>
       <c r="D37" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C38" s="2"/>
+      <c r="A38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="C38"/>
+      <c r="D38" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B39" s="1">
-        <f>B34/B33</f>
-        <v>1</v>
-      </c>
       <c r="C39" s="2"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B40" s="1">
-        <f>0.3069*LN(B39)+0.548</f>
-        <v>0.54800000000000004</v>
+        <f>B35/B34</f>
+        <v>1</v>
       </c>
       <c r="C40" s="2"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="1">
+        <f>0.3069*LN(B40)+0.548</f>
+        <v>0.54800000000000004</v>
+      </c>
       <c r="C41" s="2"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C42" s="2"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B43" s="2">
-        <f>B40*B32*B33*(1-B37^2)/B36</f>
-        <v>1.4960400000000002E-2</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="C43" s="2"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="B44" s="2">
-        <f>B43*100</f>
-        <v>1.4960400000000003</v>
+        <f>B41*B33*B34*(1-B38^2)/B37</f>
+        <v>1.4960400000000002E-2</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="2">
-        <f>B43*1000</f>
-        <v>14.960400000000002</v>
+        <f>B44*100</f>
+        <v>1.4960400000000003</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C46" s="2"/>
+      <c r="B46" s="2">
+        <f>B44*1000</f>
+        <v>14.960400000000002</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C47" s="2"/>
@@ -5857,8 +5862,12 @@
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C48" s="2"/>
     </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C49" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>